<commit_message>
updated to PS sheet to do multi-select
</commit_message>
<xml_diff>
--- a/P+C_Product_Specific_Questions_15Oct2025.xlsx
+++ b/P+C_Product_Specific_Questions_15Oct2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficorp-my.sharepoint.com/personal/markeastwood_fico_com/Documents/Documents/Global_Solution_Arch/NS Clarity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficorp-my.sharepoint.com/personal/markeastwood_fico_com/Documents/Documents/Global_Solution_Arch/Clarity_EFS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{3B5BC727-9129-6148-9F64-B356A7B1B146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -7125,29 +7125,62 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="71" fillId="5" borderId="86" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="5" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="16" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="17" borderId="42" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="17" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="17" borderId="43" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="78" fillId="17" borderId="42" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="17" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="17" borderId="43" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="5" borderId="86" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="5" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="71" fillId="5" borderId="72" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="16" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="71" fillId="5" borderId="71" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="5" borderId="109" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="97" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="85" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="84" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="72" fillId="0" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="71" fillId="5" borderId="104" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7166,39 +7199,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="88" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="84" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="85" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="72" fillId="0" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="5" borderId="72" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="5" borderId="71" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="5" borderId="109" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="97" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="3" borderId="34" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -18059,16 +18059,16 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="547" t="s">
+      <c r="A2" s="543" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="548"/>
-      <c r="C2" s="548"/>
-      <c r="D2" s="548"/>
-      <c r="E2" s="548"/>
-      <c r="F2" s="548"/>
-      <c r="G2" s="548"/>
-      <c r="H2" s="548"/>
+      <c r="B2" s="544"/>
+      <c r="C2" s="544"/>
+      <c r="D2" s="544"/>
+      <c r="E2" s="544"/>
+      <c r="F2" s="544"/>
+      <c r="G2" s="544"/>
+      <c r="H2" s="544"/>
     </row>
     <row r="3" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="370" t="s">
@@ -18105,10 +18105,10 @@
       <c r="A4" s="376" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="549"/>
-      <c r="C4" s="549"/>
-      <c r="D4" s="549"/>
-      <c r="E4" s="549"/>
+      <c r="B4" s="545"/>
+      <c r="C4" s="545"/>
+      <c r="D4" s="545"/>
+      <c r="E4" s="545"/>
       <c r="F4" s="377"/>
       <c r="G4" s="377"/>
       <c r="H4" s="378"/>
@@ -18122,12 +18122,12 @@
       <c r="A5" s="376" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="550" t="s">
+      <c r="B5" s="546" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="550"/>
-      <c r="D5" s="550"/>
-      <c r="E5" s="550"/>
+      <c r="C5" s="546"/>
+      <c r="D5" s="546"/>
+      <c r="E5" s="546"/>
       <c r="F5" s="380"/>
       <c r="G5" s="381"/>
       <c r="H5" s="382"/>
@@ -18138,26 +18138,26 @@
       <c r="M5" s="74"/>
     </row>
     <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="544" t="s">
+      <c r="A6" s="547" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="545"/>
-      <c r="C6" s="545"/>
-      <c r="D6" s="545"/>
-      <c r="E6" s="545"/>
-      <c r="F6" s="545"/>
-      <c r="G6" s="545"/>
-      <c r="H6" s="546"/>
+      <c r="B6" s="548"/>
+      <c r="C6" s="548"/>
+      <c r="D6" s="548"/>
+      <c r="E6" s="548"/>
+      <c r="F6" s="548"/>
+      <c r="G6" s="548"/>
+      <c r="H6" s="549"/>
       <c r="J6" s="375"/>
     </row>
     <row r="7" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="383" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="543"/>
-      <c r="C7" s="543"/>
-      <c r="D7" s="543"/>
-      <c r="E7" s="543"/>
+      <c r="B7" s="550"/>
+      <c r="C7" s="550"/>
+      <c r="D7" s="550"/>
+      <c r="E7" s="550"/>
       <c r="F7" s="385"/>
       <c r="G7" s="386" t="s">
         <v>122</v>
@@ -18170,12 +18170,12 @@
       <c r="A8" s="388" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="543">
+      <c r="B8" s="550">
         <v>1</v>
       </c>
-      <c r="C8" s="543"/>
-      <c r="D8" s="543"/>
-      <c r="E8" s="543"/>
+      <c r="C8" s="550"/>
+      <c r="D8" s="550"/>
+      <c r="E8" s="550"/>
       <c r="F8" s="389"/>
       <c r="G8" s="386">
         <v>1</v>
@@ -18188,12 +18188,12 @@
       <c r="A9" s="391" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="543">
+      <c r="B9" s="550">
         <v>1</v>
       </c>
-      <c r="C9" s="543"/>
-      <c r="D9" s="543"/>
-      <c r="E9" s="543"/>
+      <c r="C9" s="550"/>
+      <c r="D9" s="550"/>
+      <c r="E9" s="550"/>
       <c r="F9" s="389"/>
       <c r="G9" s="422" t="s">
         <v>127</v>
@@ -18209,12 +18209,12 @@
       <c r="A10" s="388" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="543">
+      <c r="B10" s="550">
         <v>1</v>
       </c>
-      <c r="C10" s="543"/>
-      <c r="D10" s="543"/>
-      <c r="E10" s="543"/>
+      <c r="C10" s="550"/>
+      <c r="D10" s="550"/>
+      <c r="E10" s="550"/>
       <c r="F10" s="389"/>
       <c r="G10" s="386">
         <v>1</v>
@@ -18227,16 +18227,16 @@
       <c r="L10" s="364"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="544" t="s">
+      <c r="A11" s="547" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="545"/>
-      <c r="C11" s="545"/>
-      <c r="D11" s="545"/>
-      <c r="E11" s="545"/>
-      <c r="F11" s="545"/>
-      <c r="G11" s="545"/>
-      <c r="H11" s="546"/>
+      <c r="B11" s="548"/>
+      <c r="C11" s="548"/>
+      <c r="D11" s="548"/>
+      <c r="E11" s="548"/>
+      <c r="F11" s="548"/>
+      <c r="G11" s="548"/>
+      <c r="H11" s="549"/>
       <c r="J11" s="392"/>
       <c r="K11" s="364"/>
       <c r="L11" s="364"/>
@@ -18354,16 +18354,16 @@
       <c r="L17" s="364"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="544" t="s">
+      <c r="A18" s="547" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="545"/>
-      <c r="C18" s="545"/>
-      <c r="D18" s="545"/>
-      <c r="E18" s="545"/>
-      <c r="F18" s="545"/>
-      <c r="G18" s="545"/>
-      <c r="H18" s="546"/>
+      <c r="B18" s="548"/>
+      <c r="C18" s="548"/>
+      <c r="D18" s="548"/>
+      <c r="E18" s="548"/>
+      <c r="F18" s="548"/>
+      <c r="G18" s="548"/>
+      <c r="H18" s="549"/>
       <c r="J18" s="392"/>
       <c r="K18" s="364"/>
       <c r="L18" s="364"/>
@@ -18706,16 +18706,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A18:H18"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:B30 B7:B10 B12:B17" xr:uid="{845D3C43-F911-4EF9-83FF-78705E7515D1}">
@@ -18757,19 +18757,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="551" t="s">
+      <c r="A2" s="562" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="552"/>
-      <c r="C2" s="552"/>
-      <c r="D2" s="552"/>
-      <c r="E2" s="552"/>
-      <c r="F2" s="552"/>
-      <c r="G2" s="552"/>
-      <c r="H2" s="552"/>
-      <c r="I2" s="552"/>
-      <c r="J2" s="552"/>
-      <c r="K2" s="553"/>
+      <c r="B2" s="563"/>
+      <c r="C2" s="563"/>
+      <c r="D2" s="563"/>
+      <c r="E2" s="563"/>
+      <c r="F2" s="563"/>
+      <c r="G2" s="563"/>
+      <c r="H2" s="563"/>
+      <c r="I2" s="563"/>
+      <c r="J2" s="563"/>
+      <c r="K2" s="564"/>
     </row>
     <row r="3" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="370" t="s">
@@ -18810,13 +18810,13 @@
       <c r="A4" s="466" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="554"/>
-      <c r="C4" s="554"/>
-      <c r="D4" s="554"/>
-      <c r="E4" s="554"/>
-      <c r="F4" s="554"/>
-      <c r="G4" s="554"/>
-      <c r="H4" s="554"/>
+      <c r="B4" s="565"/>
+      <c r="C4" s="565"/>
+      <c r="D4" s="565"/>
+      <c r="E4" s="565"/>
+      <c r="F4" s="565"/>
+      <c r="G4" s="565"/>
+      <c r="H4" s="565"/>
       <c r="I4" s="467"/>
       <c r="J4" s="467"/>
       <c r="K4" s="468"/>
@@ -18825,47 +18825,47 @@
       <c r="A5" s="469" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="555" t="s">
+      <c r="B5" s="566" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="556"/>
-      <c r="D5" s="556"/>
-      <c r="E5" s="556"/>
-      <c r="F5" s="556"/>
-      <c r="G5" s="556"/>
-      <c r="H5" s="556"/>
+      <c r="C5" s="567"/>
+      <c r="D5" s="567"/>
+      <c r="E5" s="567"/>
+      <c r="F5" s="567"/>
+      <c r="G5" s="567"/>
+      <c r="H5" s="567"/>
       <c r="I5" s="470"/>
       <c r="J5" s="470"/>
       <c r="K5" s="471"/>
     </row>
     <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="544" t="s">
+      <c r="A6" s="547" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="545"/>
-      <c r="C6" s="545"/>
-      <c r="D6" s="545"/>
-      <c r="E6" s="545"/>
-      <c r="F6" s="545"/>
-      <c r="G6" s="545"/>
-      <c r="H6" s="545"/>
-      <c r="I6" s="545"/>
-      <c r="J6" s="545"/>
-      <c r="K6" s="546"/>
+      <c r="B6" s="548"/>
+      <c r="C6" s="548"/>
+      <c r="D6" s="548"/>
+      <c r="E6" s="548"/>
+      <c r="F6" s="548"/>
+      <c r="G6" s="548"/>
+      <c r="H6" s="548"/>
+      <c r="I6" s="548"/>
+      <c r="J6" s="548"/>
+      <c r="K6" s="549"/>
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="456" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="557">
+      <c r="B7" s="560">
         <v>1</v>
       </c>
-      <c r="C7" s="557"/>
-      <c r="D7" s="557"/>
-      <c r="E7" s="557"/>
-      <c r="F7" s="557"/>
-      <c r="G7" s="557"/>
-      <c r="H7" s="557"/>
+      <c r="C7" s="560"/>
+      <c r="D7" s="560"/>
+      <c r="E7" s="560"/>
+      <c r="F7" s="560"/>
+      <c r="G7" s="560"/>
+      <c r="H7" s="560"/>
       <c r="I7" s="458"/>
       <c r="J7" s="459" t="s">
         <v>207</v>
@@ -18878,15 +18878,15 @@
       <c r="A8" s="461" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="543">
+      <c r="B8" s="550">
         <v>1</v>
       </c>
-      <c r="C8" s="543"/>
-      <c r="D8" s="543"/>
-      <c r="E8" s="543"/>
-      <c r="F8" s="543"/>
-      <c r="G8" s="543"/>
-      <c r="H8" s="543"/>
+      <c r="C8" s="550"/>
+      <c r="D8" s="550"/>
+      <c r="E8" s="550"/>
+      <c r="F8" s="550"/>
+      <c r="G8" s="550"/>
+      <c r="H8" s="550"/>
       <c r="I8" s="436"/>
       <c r="J8" s="386">
         <v>1</v>
@@ -18899,15 +18899,15 @@
       <c r="A9" s="462" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="543">
+      <c r="B9" s="550">
         <v>1</v>
       </c>
-      <c r="C9" s="543"/>
-      <c r="D9" s="543"/>
-      <c r="E9" s="543"/>
-      <c r="F9" s="543"/>
-      <c r="G9" s="543"/>
-      <c r="H9" s="543"/>
+      <c r="C9" s="550"/>
+      <c r="D9" s="550"/>
+      <c r="E9" s="550"/>
+      <c r="F9" s="550"/>
+      <c r="G9" s="550"/>
+      <c r="H9" s="550"/>
       <c r="I9" s="436"/>
       <c r="J9" s="422" t="s">
         <v>127</v>
@@ -18920,15 +18920,15 @@
       <c r="A10" s="463" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="558">
+      <c r="B10" s="559">
         <v>1</v>
       </c>
-      <c r="C10" s="558"/>
-      <c r="D10" s="558"/>
-      <c r="E10" s="558"/>
-      <c r="F10" s="558"/>
-      <c r="G10" s="558"/>
-      <c r="H10" s="558"/>
+      <c r="C10" s="559"/>
+      <c r="D10" s="559"/>
+      <c r="E10" s="559"/>
+      <c r="F10" s="559"/>
+      <c r="G10" s="559"/>
+      <c r="H10" s="559"/>
       <c r="I10" s="464"/>
       <c r="J10" s="465">
         <v>1</v>
@@ -18938,19 +18938,19 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="544" t="s">
+      <c r="A11" s="547" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="545"/>
-      <c r="C11" s="545"/>
-      <c r="D11" s="545"/>
-      <c r="E11" s="545"/>
-      <c r="F11" s="545"/>
-      <c r="G11" s="545"/>
-      <c r="H11" s="545"/>
-      <c r="I11" s="545"/>
-      <c r="J11" s="545"/>
-      <c r="K11" s="545"/>
+      <c r="B11" s="548"/>
+      <c r="C11" s="548"/>
+      <c r="D11" s="548"/>
+      <c r="E11" s="548"/>
+      <c r="F11" s="548"/>
+      <c r="G11" s="548"/>
+      <c r="H11" s="548"/>
+      <c r="I11" s="548"/>
+      <c r="J11" s="548"/>
+      <c r="K11" s="548"/>
     </row>
     <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="472" t="s">
@@ -19107,33 +19107,33 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="544" t="s">
+      <c r="A18" s="547" t="s">
         <v>220</v>
       </c>
-      <c r="B18" s="545"/>
-      <c r="C18" s="545"/>
-      <c r="D18" s="545"/>
-      <c r="E18" s="545"/>
-      <c r="F18" s="545"/>
-      <c r="G18" s="545"/>
-      <c r="H18" s="545"/>
-      <c r="I18" s="545"/>
-      <c r="J18" s="545"/>
-      <c r="K18" s="546"/>
+      <c r="B18" s="548"/>
+      <c r="C18" s="548"/>
+      <c r="D18" s="548"/>
+      <c r="E18" s="548"/>
+      <c r="F18" s="548"/>
+      <c r="G18" s="548"/>
+      <c r="H18" s="548"/>
+      <c r="I18" s="548"/>
+      <c r="J18" s="548"/>
+      <c r="K18" s="549"/>
     </row>
     <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="456" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="557" t="s">
+      <c r="B19" s="560" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="557"/>
-      <c r="D19" s="557"/>
-      <c r="E19" s="557"/>
-      <c r="F19" s="557"/>
-      <c r="G19" s="557"/>
-      <c r="H19" s="557"/>
+      <c r="C19" s="560"/>
+      <c r="D19" s="560"/>
+      <c r="E19" s="560"/>
+      <c r="F19" s="560"/>
+      <c r="G19" s="560"/>
+      <c r="H19" s="560"/>
       <c r="I19" s="458"/>
       <c r="J19" s="478" t="s">
         <v>221</v>
@@ -19146,13 +19146,13 @@
       <c r="A20" s="462" t="s">
         <v>223</v>
       </c>
-      <c r="B20" s="559"/>
-      <c r="C20" s="559"/>
-      <c r="D20" s="559"/>
-      <c r="E20" s="559"/>
-      <c r="F20" s="559"/>
-      <c r="G20" s="559"/>
-      <c r="H20" s="559"/>
+      <c r="B20" s="561"/>
+      <c r="C20" s="561"/>
+      <c r="D20" s="561"/>
+      <c r="E20" s="561"/>
+      <c r="F20" s="561"/>
+      <c r="G20" s="561"/>
+      <c r="H20" s="561"/>
       <c r="I20" s="438"/>
       <c r="J20" s="402" t="s">
         <v>150</v>
@@ -19165,13 +19165,13 @@
       <c r="A21" s="462" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="543"/>
-      <c r="C21" s="543"/>
-      <c r="D21" s="543"/>
-      <c r="E21" s="543"/>
-      <c r="F21" s="543"/>
-      <c r="G21" s="543"/>
-      <c r="H21" s="543"/>
+      <c r="B21" s="550"/>
+      <c r="C21" s="550"/>
+      <c r="D21" s="550"/>
+      <c r="E21" s="550"/>
+      <c r="F21" s="550"/>
+      <c r="G21" s="550"/>
+      <c r="H21" s="550"/>
       <c r="I21" s="436"/>
       <c r="J21" s="386" t="s">
         <v>153</v>
@@ -19184,13 +19184,13 @@
       <c r="A22" s="462" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="543"/>
-      <c r="C22" s="543"/>
-      <c r="D22" s="543"/>
-      <c r="E22" s="543"/>
-      <c r="F22" s="543"/>
-      <c r="G22" s="543"/>
-      <c r="H22" s="543"/>
+      <c r="B22" s="550"/>
+      <c r="C22" s="550"/>
+      <c r="D22" s="550"/>
+      <c r="E22" s="550"/>
+      <c r="F22" s="550"/>
+      <c r="G22" s="550"/>
+      <c r="H22" s="550"/>
       <c r="I22" s="436"/>
       <c r="J22" s="386" t="s">
         <v>156</v>
@@ -19203,13 +19203,13 @@
       <c r="A23" s="462" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="543"/>
-      <c r="C23" s="543"/>
-      <c r="D23" s="543"/>
-      <c r="E23" s="543"/>
-      <c r="F23" s="543"/>
-      <c r="G23" s="543"/>
-      <c r="H23" s="543"/>
+      <c r="B23" s="550"/>
+      <c r="C23" s="550"/>
+      <c r="D23" s="550"/>
+      <c r="E23" s="550"/>
+      <c r="F23" s="550"/>
+      <c r="G23" s="550"/>
+      <c r="H23" s="550"/>
       <c r="I23" s="436"/>
       <c r="J23" s="386" t="s">
         <v>156</v>
@@ -19222,15 +19222,15 @@
       <c r="A24" s="462" t="s">
         <v>160</v>
       </c>
-      <c r="B24" s="543">
+      <c r="B24" s="550">
         <v>12</v>
       </c>
-      <c r="C24" s="543"/>
-      <c r="D24" s="543"/>
-      <c r="E24" s="543"/>
-      <c r="F24" s="543"/>
-      <c r="G24" s="543"/>
-      <c r="H24" s="543"/>
+      <c r="C24" s="550"/>
+      <c r="D24" s="550"/>
+      <c r="E24" s="550"/>
+      <c r="F24" s="550"/>
+      <c r="G24" s="550"/>
+      <c r="H24" s="550"/>
       <c r="I24" s="436"/>
       <c r="J24" s="386" t="s">
         <v>226</v>
@@ -19262,13 +19262,13 @@
       <c r="A26" s="462" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="543"/>
-      <c r="C26" s="543"/>
-      <c r="D26" s="543"/>
-      <c r="E26" s="543"/>
-      <c r="F26" s="543"/>
-      <c r="G26" s="543"/>
-      <c r="H26" s="543"/>
+      <c r="B26" s="550"/>
+      <c r="C26" s="550"/>
+      <c r="D26" s="550"/>
+      <c r="E26" s="550"/>
+      <c r="F26" s="550"/>
+      <c r="G26" s="550"/>
+      <c r="H26" s="550"/>
       <c r="I26" s="436"/>
       <c r="J26" s="386" t="s">
         <v>227</v>
@@ -19319,13 +19319,13 @@
       <c r="A29" s="461" t="s">
         <v>178</v>
       </c>
-      <c r="B29" s="543"/>
-      <c r="C29" s="543"/>
-      <c r="D29" s="543"/>
-      <c r="E29" s="543"/>
-      <c r="F29" s="543"/>
-      <c r="G29" s="543"/>
-      <c r="H29" s="543"/>
+      <c r="B29" s="550"/>
+      <c r="C29" s="550"/>
+      <c r="D29" s="550"/>
+      <c r="E29" s="550"/>
+      <c r="F29" s="550"/>
+      <c r="G29" s="550"/>
+      <c r="H29" s="550"/>
       <c r="I29" s="436"/>
       <c r="J29" s="386" t="s">
         <v>179</v>
@@ -19338,13 +19338,13 @@
       <c r="A30" s="461" t="s">
         <v>181</v>
       </c>
-      <c r="B30" s="560"/>
-      <c r="C30" s="560"/>
-      <c r="D30" s="560"/>
-      <c r="E30" s="560"/>
-      <c r="F30" s="560"/>
-      <c r="G30" s="560"/>
-      <c r="H30" s="560"/>
+      <c r="B30" s="551"/>
+      <c r="C30" s="551"/>
+      <c r="D30" s="551"/>
+      <c r="E30" s="551"/>
+      <c r="F30" s="551"/>
+      <c r="G30" s="551"/>
+      <c r="H30" s="551"/>
       <c r="I30" s="439"/>
       <c r="J30" s="440" t="s">
         <v>182</v>
@@ -19357,15 +19357,15 @@
       <c r="A31" s="461" t="s">
         <v>230</v>
       </c>
-      <c r="B31" s="564" t="s">
+      <c r="B31" s="555" t="s">
         <v>231</v>
       </c>
-      <c r="C31" s="565"/>
-      <c r="D31" s="565"/>
-      <c r="E31" s="565"/>
-      <c r="F31" s="565"/>
-      <c r="G31" s="565"/>
-      <c r="H31" s="566"/>
+      <c r="C31" s="556"/>
+      <c r="D31" s="556"/>
+      <c r="E31" s="556"/>
+      <c r="F31" s="556"/>
+      <c r="G31" s="556"/>
+      <c r="H31" s="557"/>
       <c r="I31" s="436"/>
       <c r="J31" s="386"/>
       <c r="K31" s="90" t="s">
@@ -19376,15 +19376,15 @@
       <c r="A32" s="461" t="s">
         <v>232</v>
       </c>
-      <c r="B32" s="560" t="s">
+      <c r="B32" s="551" t="s">
         <v>216</v>
       </c>
-      <c r="C32" s="560"/>
-      <c r="D32" s="560"/>
-      <c r="E32" s="560"/>
-      <c r="F32" s="560"/>
-      <c r="G32" s="560"/>
-      <c r="H32" s="560"/>
+      <c r="C32" s="551"/>
+      <c r="D32" s="551"/>
+      <c r="E32" s="551"/>
+      <c r="F32" s="551"/>
+      <c r="G32" s="551"/>
+      <c r="H32" s="551"/>
       <c r="I32" s="439"/>
       <c r="J32" s="447" t="s">
         <v>233</v>
@@ -19397,15 +19397,15 @@
       <c r="A33" s="461" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="543" t="s">
+      <c r="B33" s="550" t="s">
         <v>216</v>
       </c>
-      <c r="C33" s="543"/>
-      <c r="D33" s="543"/>
-      <c r="E33" s="543"/>
-      <c r="F33" s="543"/>
-      <c r="G33" s="543"/>
-      <c r="H33" s="543"/>
+      <c r="C33" s="550"/>
+      <c r="D33" s="550"/>
+      <c r="E33" s="550"/>
+      <c r="F33" s="550"/>
+      <c r="G33" s="550"/>
+      <c r="H33" s="550"/>
       <c r="I33" s="436"/>
       <c r="J33" s="422" t="s">
         <v>235</v>
@@ -19418,13 +19418,13 @@
       <c r="A34" s="462" t="s">
         <v>193</v>
       </c>
-      <c r="B34" s="560"/>
-      <c r="C34" s="560"/>
-      <c r="D34" s="560"/>
-      <c r="E34" s="560"/>
-      <c r="F34" s="560"/>
-      <c r="G34" s="560"/>
-      <c r="H34" s="560"/>
+      <c r="B34" s="551"/>
+      <c r="C34" s="551"/>
+      <c r="D34" s="551"/>
+      <c r="E34" s="551"/>
+      <c r="F34" s="551"/>
+      <c r="G34" s="551"/>
+      <c r="H34" s="551"/>
       <c r="I34" s="439"/>
       <c r="J34" s="416" t="s">
         <v>194</v>
@@ -19437,15 +19437,15 @@
       <c r="A35" s="463" t="s">
         <v>238</v>
       </c>
-      <c r="B35" s="567" t="s">
+      <c r="B35" s="558" t="s">
         <v>216</v>
       </c>
-      <c r="C35" s="567"/>
-      <c r="D35" s="567"/>
-      <c r="E35" s="567"/>
-      <c r="F35" s="567"/>
-      <c r="G35" s="567"/>
-      <c r="H35" s="567"/>
+      <c r="C35" s="558"/>
+      <c r="D35" s="558"/>
+      <c r="E35" s="558"/>
+      <c r="F35" s="558"/>
+      <c r="G35" s="558"/>
+      <c r="H35" s="558"/>
       <c r="I35" s="479"/>
       <c r="J35" s="480"/>
       <c r="K35" s="91"/>
@@ -19463,19 +19463,19 @@
       <c r="J36" s="159"/>
     </row>
     <row r="37" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="544" t="s">
+      <c r="A37" s="547" t="s">
         <v>239</v>
       </c>
-      <c r="B37" s="545"/>
-      <c r="C37" s="545"/>
-      <c r="D37" s="545"/>
-      <c r="E37" s="545"/>
-      <c r="F37" s="545"/>
-      <c r="G37" s="545"/>
-      <c r="H37" s="545"/>
-      <c r="I37" s="545"/>
-      <c r="J37" s="545"/>
-      <c r="K37" s="546"/>
+      <c r="B37" s="548"/>
+      <c r="C37" s="548"/>
+      <c r="D37" s="548"/>
+      <c r="E37" s="548"/>
+      <c r="F37" s="548"/>
+      <c r="G37" s="548"/>
+      <c r="H37" s="548"/>
+      <c r="I37" s="548"/>
+      <c r="J37" s="548"/>
+      <c r="K37" s="549"/>
     </row>
     <row r="38" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="481" t="s">
@@ -19731,15 +19731,15 @@
       <c r="A48" s="486" t="s">
         <v>256</v>
       </c>
-      <c r="B48" s="560" t="s">
+      <c r="B48" s="551" t="s">
         <v>216</v>
       </c>
-      <c r="C48" s="560"/>
-      <c r="D48" s="560"/>
-      <c r="E48" s="560"/>
-      <c r="F48" s="560"/>
-      <c r="G48" s="560"/>
-      <c r="H48" s="560"/>
+      <c r="C48" s="551"/>
+      <c r="D48" s="551"/>
+      <c r="E48" s="551"/>
+      <c r="F48" s="551"/>
+      <c r="G48" s="551"/>
+      <c r="H48" s="551"/>
       <c r="I48" s="439"/>
       <c r="J48" s="405"/>
       <c r="K48" s="90" t="s">
@@ -19750,13 +19750,13 @@
       <c r="A49" s="486" t="s">
         <v>258</v>
       </c>
-      <c r="B49" s="560"/>
-      <c r="C49" s="560"/>
-      <c r="D49" s="560"/>
-      <c r="E49" s="560"/>
-      <c r="F49" s="560"/>
-      <c r="G49" s="560"/>
-      <c r="H49" s="560"/>
+      <c r="B49" s="551"/>
+      <c r="C49" s="551"/>
+      <c r="D49" s="551"/>
+      <c r="E49" s="551"/>
+      <c r="F49" s="551"/>
+      <c r="G49" s="551"/>
+      <c r="H49" s="551"/>
       <c r="I49" s="439"/>
       <c r="J49" s="405"/>
       <c r="K49" s="90" t="s">
@@ -19767,15 +19767,15 @@
       <c r="A50" s="486" t="s">
         <v>260</v>
       </c>
-      <c r="B50" s="560" t="s">
+      <c r="B50" s="551" t="s">
         <v>216</v>
       </c>
-      <c r="C50" s="560"/>
-      <c r="D50" s="560"/>
-      <c r="E50" s="560"/>
-      <c r="F50" s="560"/>
-      <c r="G50" s="560"/>
-      <c r="H50" s="560"/>
+      <c r="C50" s="551"/>
+      <c r="D50" s="551"/>
+      <c r="E50" s="551"/>
+      <c r="F50" s="551"/>
+      <c r="G50" s="551"/>
+      <c r="H50" s="551"/>
       <c r="I50" s="445"/>
       <c r="J50" s="446"/>
       <c r="K50" s="90"/>
@@ -19784,15 +19784,15 @@
       <c r="A51" s="462" t="s">
         <v>261</v>
       </c>
-      <c r="B51" s="560" t="s">
+      <c r="B51" s="551" t="s">
         <v>216</v>
       </c>
-      <c r="C51" s="560"/>
-      <c r="D51" s="560"/>
-      <c r="E51" s="560"/>
-      <c r="F51" s="560"/>
-      <c r="G51" s="560"/>
-      <c r="H51" s="560"/>
+      <c r="C51" s="551"/>
+      <c r="D51" s="551"/>
+      <c r="E51" s="551"/>
+      <c r="F51" s="551"/>
+      <c r="G51" s="551"/>
+      <c r="H51" s="551"/>
       <c r="I51" s="439"/>
       <c r="J51" s="405" t="s">
         <v>262</v>
@@ -19805,15 +19805,15 @@
       <c r="A52" s="462" t="s">
         <v>264</v>
       </c>
-      <c r="B52" s="560" t="s">
+      <c r="B52" s="551" t="s">
         <v>216</v>
       </c>
-      <c r="C52" s="560"/>
-      <c r="D52" s="560"/>
-      <c r="E52" s="560"/>
-      <c r="F52" s="560"/>
-      <c r="G52" s="560"/>
-      <c r="H52" s="560"/>
+      <c r="C52" s="551"/>
+      <c r="D52" s="551"/>
+      <c r="E52" s="551"/>
+      <c r="F52" s="551"/>
+      <c r="G52" s="551"/>
+      <c r="H52" s="551"/>
       <c r="I52" s="439"/>
       <c r="J52" s="405"/>
       <c r="K52" s="90"/>
@@ -19822,15 +19822,15 @@
       <c r="A53" s="367" t="s">
         <v>265</v>
       </c>
-      <c r="B53" s="560" t="s">
+      <c r="B53" s="551" t="s">
         <v>266</v>
       </c>
-      <c r="C53" s="560"/>
-      <c r="D53" s="560"/>
-      <c r="E53" s="560"/>
-      <c r="F53" s="560"/>
-      <c r="G53" s="560"/>
-      <c r="H53" s="560"/>
+      <c r="C53" s="551"/>
+      <c r="D53" s="551"/>
+      <c r="E53" s="551"/>
+      <c r="F53" s="551"/>
+      <c r="G53" s="551"/>
+      <c r="H53" s="551"/>
       <c r="I53" s="439"/>
       <c r="J53" s="405"/>
       <c r="K53" s="90" t="s">
@@ -19841,16 +19841,16 @@
       <c r="A54" s="481" t="s">
         <v>268</v>
       </c>
-      <c r="B54" s="561"/>
-      <c r="C54" s="562"/>
-      <c r="D54" s="562"/>
-      <c r="E54" s="562"/>
-      <c r="F54" s="562"/>
-      <c r="G54" s="562"/>
-      <c r="H54" s="562"/>
-      <c r="I54" s="562"/>
-      <c r="J54" s="562"/>
-      <c r="K54" s="563"/>
+      <c r="B54" s="552"/>
+      <c r="C54" s="553"/>
+      <c r="D54" s="553"/>
+      <c r="E54" s="553"/>
+      <c r="F54" s="553"/>
+      <c r="G54" s="553"/>
+      <c r="H54" s="553"/>
+      <c r="I54" s="553"/>
+      <c r="J54" s="553"/>
+      <c r="K54" s="554"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="367" t="s">
@@ -20063,6 +20063,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B29:H29"/>
     <mergeCell ref="B53:H53"/>
     <mergeCell ref="A11:K11"/>
     <mergeCell ref="B54:K54"/>
@@ -20079,22 +20095,6 @@
     <mergeCell ref="B34:H34"/>
     <mergeCell ref="B35:H35"/>
     <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="B7:H7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:H30" xr:uid="{BDA3C738-DB0D-4807-86BA-F0D8512AB18D}"/>
@@ -20662,22 +20662,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1ac1fa6a-32ec-4026-9582-9a94c50ddcb1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxKeywordTaxHTField xmlns="1ac1fa6a-32ec-4026-9582-9a94c50ddcb1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <currentlyout_x002d_facing xmlns="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360" xsi:nil="true"/>
-    <inuserguide xmlns="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010057772DF15DB03446B54B10202D66ECC3" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="79ddf04d19271d7071197b0fe9510b3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360" xmlns:ns3="1ac1fa6a-32ec-4026-9582-9a94c50ddcb1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="274e68aad00ec84b88c26c1a9e64aeab" ns2:_="" ns3:_="">
     <xsd:import namespace="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360"/>
@@ -20944,6 +20928,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1ac1fa6a-32ec-4026-9582-9a94c50ddcb1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxKeywordTaxHTField xmlns="1ac1fa6a-32ec-4026-9582-9a94c50ddcb1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <currentlyout_x002d_facing xmlns="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360" xsi:nil="true"/>
+    <inuserguide xmlns="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -20954,23 +20954,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CA2D25-5EC7-4A8B-87F3-D3ED2F55A65B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1ac1fa6a-32ec-4026-9582-9a94c50ddcb1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01A531BC-86CD-44CC-B100-180BD1F9C6F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20989,6 +20972,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CA2D25-5EC7-4A8B-87F3-D3ED2F55A65B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c9d4c2d1-9471-4c37-9c7b-4b20eb87a360"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1ac1fa6a-32ec-4026-9582-9a94c50ddcb1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0788860E-EFBD-4738-BB16-1419301A25C4}">
   <ds:schemaRefs>

</xml_diff>